<commit_message>
Updated microsoft products report
</commit_message>
<xml_diff>
--- a/reports/ms_products/template.xlsx
+++ b/reports/ms_products/template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc1/Documents/Connect/IM_Reports/reports/ms_products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADE8FF5-9C46-3141-9D46-0D107358EC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C28072A-4C7D-7A4F-820B-88A0FF9B5D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38420" yWindow="640" windowWidth="35840" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AQ$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AL$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Request Type</t>
   </si>
@@ -146,21 +146,6 @@
   </si>
   <si>
     <t>Customer Country</t>
-  </si>
-  <si>
-    <t>Microsoft Tier1 Domain</t>
-  </si>
-  <si>
-    <t>Microsoft Subscription ID</t>
-  </si>
-  <si>
-    <t>Microsoft Customer ID</t>
-  </si>
-  <si>
-    <t>Microsoft Order ID</t>
-  </si>
-  <si>
-    <t>Microsoft Subscription Plan</t>
   </si>
   <si>
     <t>Microsoft Tier1 MPN</t>
@@ -516,21 +501,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AT1"/>
+  <dimension ref="A1:AL1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AQ1" sqref="AQ1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="32" width="25" customWidth="1"/>
-    <col min="33" max="37" width="36.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="36.33203125" customWidth="1" collapsed="1"/>
-    <col min="39" max="43" width="36.33203125" customWidth="1"/>
+    <col min="33" max="37" width="36.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,24 +627,9 @@
       <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>42</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AQ1" xr:uid="{9A317F1F-30F8-304D-B686-05CCA5059EB3}"/>
+  <autoFilter ref="A1:AL1" xr:uid="{9A317F1F-30F8-304D-B686-05CCA5059EB3}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>